<commit_message>
hoan thanh PM KCB
</commit_message>
<xml_diff>
--- a/src/main/resources/data_KCB_XML/errors_KCB.xlsx
+++ b/src/main/resources/data_KCB_XML/errors_KCB.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>MaLK</t>
   </si>
@@ -42,6 +42,33 @@
   </si>
   <si>
     <t>Chi tiết lỗi</t>
+  </si>
+  <si>
+    <t>20251101073302227</t>
+  </si>
+  <si>
+    <t>2511020085</t>
+  </si>
+  <si>
+    <t>10.19</t>
+  </si>
+  <si>
+    <t>Khám Ngoại tổng hợp</t>
+  </si>
+  <si>
+    <t>009359/QNA-CCHN</t>
+  </si>
+  <si>
+    <t>2025-11-01 13:50</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>2025-11-01 13:54</t>
+  </si>
+  <si>
+    <t>⛔ Bác sĩ Bs.Duy Đạt nghỉ T7, không làm việc vào chỉ định: 202511011350</t>
   </si>
 </sst>
 </file>
@@ -107,22 +134,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="5.55859375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="6.49609375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="17.9296875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="10.9296875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="6.50390625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="6.83203125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="10.328125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="11.796875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="7.39453125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="18.37109375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="16.64453125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="16.64453125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="15.11328125" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="9.6171875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="7.96875" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="9.3046875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="15.11328125" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="58.45703125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -157,6 +184,38 @@
         <v>9</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
update check trung ngay YL & THYL
</commit_message>
<xml_diff>
--- a/src/main/resources/data_KCB_XML/errors_KCB.xlsx
+++ b/src/main/resources/data_KCB_XML/errors_KCB.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="62">
   <si>
     <t>MaLK</t>
   </si>
@@ -44,31 +44,160 @@
     <t>Chi tiết lỗi</t>
   </si>
   <si>
-    <t>20251101073302227</t>
-  </si>
-  <si>
-    <t>2511020085</t>
-  </si>
-  <si>
-    <t>10.19</t>
-  </si>
-  <si>
-    <t>Khám Ngoại tổng hợp</t>
-  </si>
-  <si>
-    <t>009359/QNA-CCHN</t>
-  </si>
-  <si>
-    <t>2025-11-01 13:50</t>
+    <t>20251116091706633</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>2025-11-01 13:54</t>
-  </si>
-  <si>
-    <t>⛔ Bác sĩ Bs.Duy Đạt nghỉ T7, không làm việc vào chỉ định: 202511011350</t>
+    <t>18.0004.0001</t>
+  </si>
+  <si>
+    <t>Siêu âm hạch vùng cổ</t>
+  </si>
+  <si>
+    <t>0034449/HCM-CCHN</t>
+  </si>
+  <si>
+    <t>001070/TB-CCHN</t>
+  </si>
+  <si>
+    <t>2025-11-16 09:35</t>
+  </si>
+  <si>
+    <t>2025-11-16 09:38</t>
+  </si>
+  <si>
+    <t>2025-11-16 09:50</t>
+  </si>
+  <si>
+    <t>Thời gian DV Siêu âm hạch vùng cổ lệch 12p, chuẩn 15-30</t>
+  </si>
+  <si>
+    <t>20251116091023833</t>
+  </si>
+  <si>
+    <t>2511020695</t>
+  </si>
+  <si>
+    <t>18.0091.0029</t>
+  </si>
+  <si>
+    <t>Chụp X-quang cột sống thắt lưng thẳng nghiêng [số hóa 2 phim]</t>
+  </si>
+  <si>
+    <t>2025-11-16 09:47</t>
+  </si>
+  <si>
+    <t>2025-11-16 09:48</t>
+  </si>
+  <si>
+    <t>2025-11-16 09:57</t>
+  </si>
+  <si>
+    <t>Bác sĩ không có chuyên môn làm DV này</t>
+  </si>
+  <si>
+    <t>20251116090838933</t>
+  </si>
+  <si>
+    <t>2504011397</t>
+  </si>
+  <si>
+    <t>18.0119.0028</t>
+  </si>
+  <si>
+    <t>Chụp X-quang ngực thẳng [số hóa 1 phim]</t>
+  </si>
+  <si>
+    <t>2025-11-16 09:24</t>
+  </si>
+  <si>
+    <t>2025-11-16 09:26</t>
+  </si>
+  <si>
+    <t>20251116090543333</t>
+  </si>
+  <si>
+    <t>2506015040</t>
+  </si>
+  <si>
+    <t>2025-11-16 09:30</t>
+  </si>
+  <si>
+    <t>2025-11-16 09:42</t>
+  </si>
+  <si>
+    <t>20251116090223010</t>
+  </si>
+  <si>
+    <t>2508016756</t>
+  </si>
+  <si>
+    <t>2025-11-16 09:44</t>
+  </si>
+  <si>
+    <t>2025-11-16 09:45</t>
+  </si>
+  <si>
+    <t>2025-11-16 09:56</t>
+  </si>
+  <si>
+    <t>20251116082510593</t>
+  </si>
+  <si>
+    <t>2412005015</t>
+  </si>
+  <si>
+    <t>18.0091.0028</t>
+  </si>
+  <si>
+    <t>Chụp X-quang cột sống thắt lưng thẳng nghiêng [số hóa 1 phim]</t>
+  </si>
+  <si>
+    <t>2025-11-16 08:39</t>
+  </si>
+  <si>
+    <t>2025-11-16 08:41</t>
+  </si>
+  <si>
+    <t>2025-11-16 08:53</t>
+  </si>
+  <si>
+    <t>20251116070851543</t>
+  </si>
+  <si>
+    <t>2508017200</t>
+  </si>
+  <si>
+    <t>2025-11-16 07:17</t>
+  </si>
+  <si>
+    <t>2025-11-16 07:20</t>
+  </si>
+  <si>
+    <t>2025-11-16 07:32</t>
+  </si>
+  <si>
+    <t>20251116070747563</t>
+  </si>
+  <si>
+    <t>2501006987</t>
+  </si>
+  <si>
+    <t>18.0112.0029</t>
+  </si>
+  <si>
+    <t>Chụp X-quang khớp gối thẳng, nghiêng hoặc chếch [số hóa 2 phim]</t>
+  </si>
+  <si>
+    <t>2025-11-16 08:05</t>
+  </si>
+  <si>
+    <t>2025-11-16 08:06</t>
+  </si>
+  <si>
+    <t>2025-11-16 08:18</t>
   </si>
 </sst>
 </file>
@@ -134,7 +263,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -142,14 +271,14 @@
   <cols>
     <col min="1" max="1" width="17.9296875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="10.9296875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="6.50390625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="18.37109375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="16.64453125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="16.64453125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.92578125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="54.37109375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="17.87109375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="14.9375" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="15.11328125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="9.6171875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="15.11328125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="15.11328125" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="58.45703125" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="46.97265625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -201,19 +330,243 @@
         <v>14</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s" s="2">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s" s="0">
         <v>16</v>
       </c>
+      <c r="H2" t="s" s="2">
+        <v>17</v>
+      </c>
       <c r="I2" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s" s="2">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="I3" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="H4" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="I4" t="s" s="2">
         <v>17</v>
       </c>
-      <c r="J2" t="s" s="0">
-        <v>18</v>
+      <c r="J4" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="H5" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="I5" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="J5" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H6" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I6" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="J6" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="G7" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="H7" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="I7" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="J7" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="G8" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="H8" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="I8" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="J8" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="G9" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="H9" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="I9" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="J9" t="s" s="0">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>